<commit_message>
algorithm list update and lightweight forms
</commit_message>
<xml_diff>
--- a/Jmetal_Algorithms .xlsx
+++ b/Jmetal_Algorithms .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Documents\GitHub\ES2-2018-LIGE-PL-82\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C16A1C-FBA8-486F-800D-2CB9EE4E6F89}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C5A287-4F9E-41E3-9BE2-A2686016A1F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{7B22BEB7-BE88-42EF-8E3B-B7A398BA13E3}"/>
   </bookViews>
@@ -656,241 +656,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B764CDD-9C87-4AAF-B8E6-67AA16063470}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="99.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -898,13 +896,13 @@
         <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -912,13 +910,13 @@
         <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -926,13 +924,13 @@
         <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -940,13 +938,13 @@
         <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,13 +952,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -968,13 +966,13 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -982,13 +980,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -996,13 +994,13 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1010,13 +1008,13 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1024,13 +1022,13 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,13 +1036,13 @@
         <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1052,13 +1050,13 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
         <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,13 +1064,13 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
         <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1080,13 +1078,13 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
         <v>22</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1094,13 +1092,13 @@
         <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
         <v>22</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1118,126 +1116,126 @@
       <c r="A35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B35" t="s">
-        <v>22</v>
+      <c r="B35" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C35" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>24</v>
+      <c r="D35" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B36" t="s">
-        <v>16</v>
+      <c r="B36" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C36" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>25</v>
+      <c r="D36" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B37" t="s">
-        <v>16</v>
+      <c r="B37" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C37" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>26</v>
+      <c r="D37" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B38" t="s">
-        <v>22</v>
+      <c r="B38" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C38" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>27</v>
+      <c r="D38" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B39" t="s">
-        <v>22</v>
+      <c r="B39" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C39" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>28</v>
+      <c r="D39" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B40" t="s">
-        <v>22</v>
+      <c r="B40" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C40" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>29</v>
+      <c r="D40" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B41" t="s">
-        <v>22</v>
+      <c r="B41" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C41" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>30</v>
+      <c r="D41" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B42" t="s">
-        <v>16</v>
+      <c r="B42" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C42" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>31</v>
+      <c r="D42" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B43" t="s">
-        <v>16</v>
+      <c r="B43" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C43" t="s">
         <v>16</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>32</v>
+      <c r="D43" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>